<commit_message>
Adding "player won" end game
still needs to be tested
</commit_message>
<xml_diff>
--- a/spritesBuildingFile.xlsx
+++ b/spritesBuildingFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MesChoses\Autres\Github\multiplayerSnake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C0FC444-85C1-4796-B5DF-966A188A9862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6BA3B5-1427-4998-8EAF-C31B994584DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CA1E80F-696C-4149-87A2-9728D32DECC1}"/>
   </bookViews>
@@ -91,7 +91,441 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="65">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -115,6 +549,13 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC00CC"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FFFFB7B7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -426,7 +867,7 @@
   <dimension ref="A1:AF32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,19 +978,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -558,43 +999,43 @@
         <v>0</v>
       </c>
       <c r="I2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
       </c>
       <c r="K2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="1">
         <v>0</v>
       </c>
       <c r="O2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" s="1">
         <v>0</v>
       </c>
       <c r="S2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2" s="1">
         <v>0</v>
@@ -635,7 +1076,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -647,46 +1088,46 @@
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
       </c>
       <c r="K3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1">
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
       </c>
       <c r="O3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
       </c>
       <c r="Q3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="1">
         <v>0</v>
       </c>
       <c r="S3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" s="1">
         <v>0</v>
@@ -733,49 +1174,49 @@
         <v>0</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
       </c>
       <c r="K4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="1">
         <v>0</v>
@@ -784,13 +1225,13 @@
         <v>0</v>
       </c>
       <c r="S4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="1">
         <v>0</v>
@@ -837,13 +1278,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -852,37 +1293,37 @@
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
       </c>
       <c r="Q5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5" s="1">
         <v>0</v>
       </c>
       <c r="S5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5" s="1">
         <v>0</v>
@@ -929,19 +1370,19 @@
         <v>0</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -950,43 +1391,43 @@
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
       </c>
       <c r="K6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="1">
         <v>0</v>
       </c>
       <c r="M6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="1">
         <v>0</v>
       </c>
       <c r="O6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" s="1">
         <v>0</v>
       </c>
       <c r="Q6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6" s="1">
         <v>0</v>
       </c>
       <c r="S6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" s="1">
         <v>0</v>
@@ -3572,11 +4013,38 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AF32">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
       <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Drafting better victory screen
</commit_message>
<xml_diff>
--- a/spritesBuildingFile.xlsx
+++ b/spritesBuildingFile.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MesChoses\Autres\Github\multiplayerSnake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327FAD9F-8C4D-48AC-9A80-A5B875FF264E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617D9E8A-C7DB-4CFB-AE83-841F0068A8C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CA1E80F-696C-4149-87A2-9728D32DECC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -91,7 +91,1778 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="275">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -566,7 +2337,7 @@
   <dimension ref="A1:AF32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="AA25" sqref="A1:AF32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,16 +2561,16 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="1">
         <v>0</v>
@@ -823,16 +2594,16 @@
         <v>0</v>
       </c>
       <c r="R3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" s="1">
         <v>0</v>
@@ -847,10 +2618,10 @@
         <v>0</v>
       </c>
       <c r="Z3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB3" s="1">
         <v>0</v>
@@ -879,7 +2650,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -888,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -897,31 +2668,31 @@
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="1">
         <v>0</v>
@@ -930,7 +2701,7 @@
         <v>0</v>
       </c>
       <c r="U4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="1">
         <v>0</v>
@@ -945,16 +2716,16 @@
         <v>0</v>
       </c>
       <c r="Z4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="1">
         <v>0</v>
       </c>
       <c r="AC4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD4" s="1">
         <v>0</v>
@@ -980,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
@@ -1028,7 +2799,7 @@
         <v>0</v>
       </c>
       <c r="U5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5" s="1">
         <v>0</v>
@@ -1043,13 +2814,13 @@
         <v>0</v>
       </c>
       <c r="Z5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC5" s="1">
         <v>0</v>
@@ -1081,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -1126,25 +2897,25 @@
         <v>0</v>
       </c>
       <c r="U6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB6" s="1">
         <v>0</v>
@@ -1170,13 +2941,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -1245,13 +3016,13 @@
         <v>0</v>
       </c>
       <c r="AB7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE7" s="1">
         <v>0</v>
@@ -1271,7 +3042,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -1369,7 +3140,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -1444,13 +3215,13 @@
         <v>0</v>
       </c>
       <c r="AC9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF9" s="1">
         <v>0</v>
@@ -1467,7 +3238,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -1482,19 +3253,19 @@
         <v>0</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" s="1">
         <v>0</v>
       </c>
       <c r="M10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N10" s="1">
         <v>0</v>
@@ -1506,25 +3277,25 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R10" s="1">
         <v>0</v>
       </c>
       <c r="S10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T10" s="1">
         <v>0</v>
       </c>
       <c r="U10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X10" s="1">
         <v>0</v>
@@ -1548,7 +3319,7 @@
         <v>0</v>
       </c>
       <c r="AE10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF10" s="1">
         <v>0</v>
@@ -1565,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -1580,19 +3351,19 @@
         <v>0</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="1">
         <v>0</v>
       </c>
       <c r="K11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L11" s="1">
         <v>0</v>
       </c>
       <c r="M11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N11" s="1">
         <v>0</v>
@@ -1604,19 +3375,19 @@
         <v>0</v>
       </c>
       <c r="Q11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R11" s="1">
         <v>0</v>
       </c>
       <c r="S11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T11" s="1">
         <v>0</v>
       </c>
       <c r="U11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V11" s="1">
         <v>0</v>
@@ -1646,7 +3417,7 @@
         <v>0</v>
       </c>
       <c r="AE11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="1">
         <v>0</v>
@@ -1663,7 +3434,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -1678,19 +3449,19 @@
         <v>0</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
@@ -1702,25 +3473,25 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R12" s="1">
         <v>0</v>
       </c>
       <c r="S12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T12" s="1">
         <v>0</v>
       </c>
       <c r="U12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X12" s="1">
         <v>0</v>
@@ -1744,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="AE12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="1">
         <v>0</v>
@@ -1755,13 +3526,13 @@
         <v>0</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -1770,64 +3541,64 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
       </c>
       <c r="K13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="1">
         <v>0</v>
       </c>
       <c r="M13" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" s="1">
         <v>0</v>
       </c>
       <c r="P13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13" s="1">
         <v>0</v>
       </c>
       <c r="X13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA13" s="1">
         <v>0</v>
@@ -1842,7 +3613,7 @@
         <v>0</v>
       </c>
       <c r="AE13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF13" s="1">
         <v>0</v>
@@ -1853,7 +3624,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -1868,58 +3639,58 @@
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="1">
         <v>0</v>
@@ -1940,7 +3711,7 @@
         <v>0</v>
       </c>
       <c r="AE14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF14" s="1">
         <v>0</v>
@@ -1951,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -1966,49 +3737,49 @@
         <v>0</v>
       </c>
       <c r="G15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="1">
         <v>0</v>
       </c>
       <c r="K15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="1">
         <v>0</v>
       </c>
       <c r="M15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15" s="1">
         <v>0</v>
       </c>
       <c r="P15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15" s="1">
         <v>0</v>
       </c>
       <c r="T15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15" s="1">
         <v>0</v>
@@ -2017,13 +3788,13 @@
         <v>0</v>
       </c>
       <c r="X15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="1">
         <v>0</v>
@@ -2038,7 +3809,7 @@
         <v>0</v>
       </c>
       <c r="AE15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF15" s="1">
         <v>0</v>
@@ -2049,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -2070,13 +3841,13 @@
         <v>0</v>
       </c>
       <c r="I16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="1">
         <v>0</v>
       </c>
       <c r="K16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="1">
         <v>0</v>
@@ -2085,37 +3856,37 @@
         <v>0</v>
       </c>
       <c r="N16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="1">
         <v>0</v>
       </c>
       <c r="P16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="1">
         <v>0</v>
       </c>
       <c r="R16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S16" s="1">
         <v>0</v>
       </c>
       <c r="T16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16" s="1">
         <v>0</v>
       </c>
       <c r="V16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W16" s="1">
         <v>0</v>
       </c>
       <c r="X16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="1">
         <v>0</v>
@@ -2136,7 +3907,7 @@
         <v>0</v>
       </c>
       <c r="AE16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF16" s="1">
         <v>0</v>
@@ -2147,7 +3918,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -2162,19 +3933,19 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="1">
         <v>0</v>
       </c>
       <c r="K17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="1">
         <v>0</v>
@@ -2183,43 +3954,43 @@
         <v>0</v>
       </c>
       <c r="N17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" s="1">
         <v>0</v>
       </c>
       <c r="P17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="1">
         <v>0</v>
       </c>
       <c r="R17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17" s="1">
         <v>0</v>
       </c>
       <c r="T17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17" s="1">
         <v>0</v>
       </c>
       <c r="V17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" s="1">
         <v>0</v>
       </c>
       <c r="X17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="1">
         <v>0</v>
@@ -2231,10 +4002,10 @@
         <v>0</v>
       </c>
       <c r="AD17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF17" s="1">
         <v>0</v>
@@ -2245,26 +4016,26 @@
         <v>0</v>
       </c>
       <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
         <v>1</v>
       </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
       <c r="I18" s="1">
         <v>0</v>
       </c>
@@ -2275,19 +4046,19 @@
         <v>0</v>
       </c>
       <c r="L18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="1">
         <v>0</v>
       </c>
       <c r="N18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="1">
         <v>0</v>
       </c>
       <c r="P18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="1">
         <v>0</v>
@@ -2296,25 +4067,25 @@
         <v>0</v>
       </c>
       <c r="S18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18" s="1">
         <v>0</v>
       </c>
       <c r="U18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X18" s="1">
         <v>0</v>
       </c>
       <c r="Y18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z18" s="1">
         <v>0</v>
@@ -2329,7 +4100,7 @@
         <v>0</v>
       </c>
       <c r="AD18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE18" s="1">
         <v>0</v>
@@ -2343,26 +4114,26 @@
         <v>0</v>
       </c>
       <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
       <c r="I19" s="1">
         <v>0</v>
       </c>
@@ -2373,34 +4144,34 @@
         <v>0</v>
       </c>
       <c r="L19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="1">
         <v>0</v>
       </c>
       <c r="N19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="1">
         <v>0</v>
       </c>
       <c r="P19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
       </c>
       <c r="S19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" s="1">
         <v>0</v>
       </c>
       <c r="U19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19" s="1">
         <v>0</v>
@@ -2412,7 +4183,7 @@
         <v>0</v>
       </c>
       <c r="Y19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z19" s="1">
         <v>0</v>
@@ -2427,7 +4198,7 @@
         <v>0</v>
       </c>
       <c r="AD19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE19" s="1">
         <v>0</v>
@@ -2441,76 +4212,76 @@
         <v>0</v>
       </c>
       <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
       <c r="I20" s="1">
         <v>0</v>
       </c>
       <c r="J20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="1">
         <v>0</v>
       </c>
       <c r="L20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="1">
         <v>0</v>
       </c>
       <c r="N20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20" s="1">
         <v>0</v>
       </c>
       <c r="P20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="1">
         <v>0</v>
       </c>
       <c r="R20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>
       </c>
       <c r="U20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
       </c>
       <c r="Y20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z20" s="1">
         <v>0</v>
@@ -2525,7 +4296,7 @@
         <v>0</v>
       </c>
       <c r="AD20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE20" s="1">
         <v>0</v>
@@ -2539,49 +4310,49 @@
         <v>0</v>
       </c>
       <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="1">
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
         <v>1</v>
       </c>
-      <c r="D21" s="1">
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1">
-        <v>0</v>
-      </c>
-      <c r="L21" s="1">
-        <v>0</v>
-      </c>
       <c r="M21" s="1">
         <v>0</v>
       </c>
       <c r="N21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" s="1">
         <v>0</v>
       </c>
       <c r="P21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="1">
         <v>0</v>
@@ -2590,19 +4361,19 @@
         <v>0</v>
       </c>
       <c r="S21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21" s="1">
+        <v>0</v>
+      </c>
+      <c r="U21" s="1">
+        <v>0</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0</v>
+      </c>
+      <c r="W21" s="1">
         <v>1</v>
-      </c>
-      <c r="U21" s="1">
-        <v>0</v>
-      </c>
-      <c r="V21" s="1">
-        <v>0</v>
-      </c>
-      <c r="W21" s="1">
-        <v>0</v>
       </c>
       <c r="X21" s="1">
         <v>0</v>
@@ -2655,31 +4426,31 @@
         <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="1">
         <v>0</v>
       </c>
       <c r="N22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22" s="1">
         <v>0</v>
       </c>
       <c r="P22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22" s="1">
         <v>0</v>
@@ -2688,25 +4459,25 @@
         <v>0</v>
       </c>
       <c r="S22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T22" s="1">
+        <v>0</v>
+      </c>
+      <c r="U22" s="1">
         <v>1</v>
       </c>
-      <c r="U22" s="1">
-        <v>0</v>
-      </c>
       <c r="V22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X22" s="1">
         <v>0</v>
       </c>
       <c r="Y22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z22" s="1">
         <v>0</v>
@@ -2789,7 +4560,7 @@
         <v>0</v>
       </c>
       <c r="T23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="1">
         <v>0</v>
@@ -2887,7 +4658,7 @@
         <v>0</v>
       </c>
       <c r="T24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U24" s="1">
         <v>0</v>
@@ -2955,19 +4726,19 @@
         <v>0</v>
       </c>
       <c r="J25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="1">
         <v>0</v>
@@ -2985,7 +4756,7 @@
         <v>0</v>
       </c>
       <c r="T25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U25" s="1">
         <v>0</v>
@@ -3032,13 +4803,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -3065,7 +4836,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" s="1">
         <v>0</v>
@@ -3083,7 +4854,7 @@
         <v>0</v>
       </c>
       <c r="T26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U26" s="1">
         <v>0</v>
@@ -3107,13 +4878,13 @@
         <v>0</v>
       </c>
       <c r="AB26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE26" s="1">
         <v>0</v>
@@ -3139,7 +4910,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27" s="1">
         <v>0</v>
@@ -3163,7 +4934,7 @@
         <v>0</v>
       </c>
       <c r="N27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O27" s="1">
         <v>0</v>
@@ -3181,7 +4952,7 @@
         <v>0</v>
       </c>
       <c r="T27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U27" s="1">
         <v>0</v>
@@ -3202,7 +4973,7 @@
         <v>0</v>
       </c>
       <c r="AA27" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB27" s="1">
         <v>0</v>
@@ -3234,13 +5005,13 @@
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
       </c>
       <c r="G28" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" s="1">
         <v>0</v>
@@ -3261,7 +5032,7 @@
         <v>0</v>
       </c>
       <c r="N28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28" s="1">
         <v>0</v>
@@ -3279,7 +5050,7 @@
         <v>0</v>
       </c>
       <c r="T28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U28" s="1">
         <v>0</v>
@@ -3297,13 +5068,13 @@
         <v>0</v>
       </c>
       <c r="Z28" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA28" s="1">
         <v>0</v>
       </c>
       <c r="AB28" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC28" s="1">
         <v>0</v>
@@ -3329,7 +5100,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -3338,7 +5109,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H29" s="1">
         <v>0</v>
@@ -3359,25 +5130,25 @@
         <v>0</v>
       </c>
       <c r="N29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U29" s="1">
         <v>0</v>
@@ -3395,7 +5166,7 @@
         <v>0</v>
       </c>
       <c r="Z29" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA29" s="1">
         <v>0</v>
@@ -3404,7 +5175,7 @@
         <v>0</v>
       </c>
       <c r="AC29" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD29" s="1">
         <v>0</v>
@@ -3436,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" s="1">
         <v>0</v>
@@ -3493,7 +5264,7 @@
         <v>0</v>
       </c>
       <c r="Z30" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA30" s="1">
         <v>0</v>
@@ -3711,7 +5482,812 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:AF11 A18:AF32 A12:F17 AA12:AF17 G13:Z17">
+  <conditionalFormatting sqref="Z18:AD21 H18:Y22 I10:W14 Y10:AD14 H14:W14 A32 A1 Z3:AD3 AD4:AD6 T7:AD7 Z4:AC7 C3:Y6 G4:G7 A3:A30 C7:E7 C8:D8 C1:AD1 C32:AD32 C22:AD30 C10:G11 C9 C12:C21 AF32 AF1 AF3:AF7 AF10:AF14 AF18:AF30">
+    <cfRule type="cellIs" dxfId="274" priority="298" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="273" priority="299" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="272" priority="300" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="271" priority="301" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="270" priority="302" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="269" priority="303" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="268" priority="304" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="267" priority="305" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="266" priority="306" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="265" priority="307" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="264" priority="308" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:G14 D18:G21 D15:E16 D17:F17">
+    <cfRule type="cellIs" dxfId="263" priority="276" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="262" priority="277" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="261" priority="278" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="260" priority="279" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="259" priority="280" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="258" priority="281" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="257" priority="282" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="256" priority="283" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="255" priority="284" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="254" priority="285" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="286" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:E8">
+    <cfRule type="cellIs" dxfId="252" priority="254" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="251" priority="255" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="250" priority="256" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="249" priority="257" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="248" priority="258" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="247" priority="259" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="246" priority="260" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="245" priority="261" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="244" priority="262" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="243" priority="263" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="242" priority="264" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:G9">
+    <cfRule type="cellIs" dxfId="241" priority="243" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="240" priority="244" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="239" priority="245" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="238" priority="246" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="237" priority="247" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="236" priority="248" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="235" priority="249" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="234" priority="250" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="233" priority="251" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="232" priority="252" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="231" priority="253" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:S7">
+    <cfRule type="cellIs" dxfId="230" priority="221" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="229" priority="222" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="228" priority="223" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="227" priority="224" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="225" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="225" priority="226" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="224" priority="227" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="223" priority="228" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="222" priority="229" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="221" priority="230" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="220" priority="231" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:AD8 AF8">
+    <cfRule type="cellIs" dxfId="219" priority="210" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="218" priority="211" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="212" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="216" priority="213" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="215" priority="214" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="215" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="213" priority="216" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="212" priority="217" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="218" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="210" priority="219" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="209" priority="220" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:AD15 AF15">
+    <cfRule type="cellIs" dxfId="208" priority="199" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="207" priority="200" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="206" priority="201" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="205" priority="202" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="204" priority="203" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="203" priority="204" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="202" priority="205" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="201" priority="206" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="200" priority="207" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="199" priority="208" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="198" priority="209" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16:AD16 AF16">
+    <cfRule type="cellIs" dxfId="197" priority="188" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="189" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="195" priority="190" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="194" priority="191" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="192" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="192" priority="193" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="191" priority="194" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="195" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="189" priority="196" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="188" priority="197" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="187" priority="198" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:I11">
+    <cfRule type="cellIs" dxfId="186" priority="177" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="185" priority="178" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="184" priority="179" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="183" priority="180" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="182" priority="181" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="181" priority="182" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="180" priority="183" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="179" priority="184" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="178" priority="185" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="177" priority="186" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="187" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="cellIs" dxfId="175" priority="166" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="174" priority="167" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="173" priority="168" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="172" priority="169" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="171" priority="170" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="170" priority="171" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="169" priority="172" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="168" priority="173" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="167" priority="174" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="175" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="165" priority="176" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="cellIs" dxfId="164" priority="155" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="163" priority="156" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="162" priority="157" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="161" priority="158" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="159" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="159" priority="160" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="161" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="162" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="156" priority="163" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="164" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="165" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="cellIs" dxfId="153" priority="144" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="152" priority="145" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="146" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="147" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="148" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="149" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="150" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="151" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="152" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="153" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="143" priority="154" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:AD17 AF17">
+    <cfRule type="cellIs" dxfId="142" priority="133" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="134" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="135" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="139" priority="136" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="137" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="138" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="139" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="135" priority="140" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="141" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="142" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="143" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T9:AD9 AF9">
+    <cfRule type="cellIs" dxfId="131" priority="122" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="123" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="124" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="125" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="126" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="127" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="128" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="129" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="130" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="131" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="132" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:S9">
+    <cfRule type="cellIs" dxfId="120" priority="111" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="112" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="113" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="114" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="115" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="116" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="117" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="118" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="119" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="111" priority="120" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="121" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X10:X14">
+    <cfRule type="cellIs" dxfId="109" priority="100" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="101" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="102" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="103" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="104" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="105" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="103" priority="106" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="107" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="108" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="109" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="110" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="cellIs" dxfId="98" priority="89" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="90" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="91" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="92" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="93" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="94" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="95" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="96" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="97" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="98" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="99" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2 C2:AD2 AF2">
+    <cfRule type="cellIs" dxfId="87" priority="78" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="79" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="80" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="81" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="82" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="83" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="84" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="85" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="86" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="87" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="88" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31 C31:AD31 AF31">
+    <cfRule type="cellIs" dxfId="76" priority="67" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="68" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="69" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="70" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="71" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="73" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="74" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="75" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="76" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="77" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32 B1 B3:B30">
+    <cfRule type="cellIs" dxfId="65" priority="56" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="57" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="58" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="59" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="60" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="63" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="64" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="65" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="66" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="cellIs" dxfId="54" priority="45" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="46" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="47" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="48" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
+    <cfRule type="cellIs" dxfId="43" priority="34" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="35" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="36" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE32 AE1 AE3:AE30">
+    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="25" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="33" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE2">
     <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
       <formula>10</formula>
     </cfRule>
@@ -3746,7 +6322,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12:Z12">
+  <conditionalFormatting sqref="AE31">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
Changing maps a bit
</commit_message>
<xml_diff>
--- a/spritesBuildingFile.xlsx
+++ b/spritesBuildingFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MesChoses\Autres\Github\multiplayerSnake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BDCB04-EF57-4141-94A3-7ED8FDC9F730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11387A6B-9273-4667-B1CF-18D720618B41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CA1E80F-696C-4149-87A2-9728D32DECC1}"/>
   </bookViews>
@@ -9347,8 +9347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412CFC93-C3A4-4E96-AFC8-C2E965482321}">
   <dimension ref="A1:AF32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10062,7 +10062,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
@@ -10074,7 +10074,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="1">
         <v>0</v>
@@ -10101,7 +10101,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="1">
         <v>0</v>
@@ -10113,7 +10113,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8" s="1">
         <v>0</v>
@@ -10160,19 +10160,19 @@
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="I9" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1">
         <v>0</v>
@@ -10199,19 +10199,19 @@
         <v>0</v>
       </c>
       <c r="T9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9" s="1">
         <v>0</v>
       </c>
       <c r="V9" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W9" s="1">
         <v>0</v>
       </c>
       <c r="X9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="1">
         <v>0</v>
@@ -10258,7 +10258,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
@@ -10270,7 +10270,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="1">
         <v>0</v>
@@ -10297,7 +10297,7 @@
         <v>0</v>
       </c>
       <c r="T10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" s="1">
         <v>0</v>
@@ -10309,7 +10309,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="1">
         <v>0</v>
@@ -10356,7 +10356,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
@@ -10368,7 +10368,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="1">
         <v>0</v>
@@ -10395,7 +10395,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" s="1">
         <v>0</v>
@@ -10407,7 +10407,7 @@
         <v>0</v>
       </c>
       <c r="X11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="1">
         <v>0</v>
@@ -10454,7 +10454,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
@@ -10466,7 +10466,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
@@ -10493,7 +10493,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" s="1">
         <v>0</v>
@@ -10505,7 +10505,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="1">
         <v>0</v>
@@ -10552,7 +10552,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
@@ -10564,7 +10564,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="1">
         <v>0</v>
@@ -10591,7 +10591,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13" s="1">
         <v>0</v>
@@ -10603,7 +10603,7 @@
         <v>0</v>
       </c>
       <c r="X13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="1">
         <v>0</v>
@@ -10650,7 +10650,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
@@ -10662,7 +10662,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="1">
         <v>0</v>
@@ -10689,7 +10689,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14" s="1">
         <v>0</v>
@@ -10701,7 +10701,7 @@
         <v>0</v>
       </c>
       <c r="X14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="1">
         <v>0</v>
@@ -10748,7 +10748,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
@@ -10760,7 +10760,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="1">
         <v>0</v>
@@ -10787,7 +10787,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" s="1">
         <v>0</v>
@@ -10799,7 +10799,7 @@
         <v>0</v>
       </c>
       <c r="X15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="1">
         <v>0</v>
@@ -10846,7 +10846,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
@@ -10858,7 +10858,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="1">
         <v>0</v>
@@ -10885,7 +10885,7 @@
         <v>0</v>
       </c>
       <c r="T16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16" s="1">
         <v>0</v>
@@ -10897,7 +10897,7 @@
         <v>0</v>
       </c>
       <c r="X16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="1">
         <v>0</v>
@@ -10944,7 +10944,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -10956,7 +10956,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="1">
         <v>0</v>
@@ -10983,7 +10983,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17" s="1">
         <v>0</v>
@@ -10995,7 +10995,7 @@
         <v>0</v>
       </c>
       <c r="X17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="1">
         <v>0</v>
@@ -11042,7 +11042,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -11054,7 +11054,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="1">
         <v>0</v>
@@ -11081,7 +11081,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U18" s="1">
         <v>0</v>
@@ -11093,7 +11093,7 @@
         <v>0</v>
       </c>
       <c r="X18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y18" s="1">
         <v>0</v>
@@ -11140,7 +11140,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
@@ -11152,7 +11152,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
@@ -11179,7 +11179,7 @@
         <v>0</v>
       </c>
       <c r="T19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19" s="1">
         <v>0</v>
@@ -11191,7 +11191,7 @@
         <v>0</v>
       </c>
       <c r="X19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="1">
         <v>0</v>
@@ -11238,7 +11238,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
@@ -11250,7 +11250,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
@@ -11277,7 +11277,7 @@
         <v>0</v>
       </c>
       <c r="T20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U20" s="1">
         <v>0</v>
@@ -11289,7 +11289,7 @@
         <v>0</v>
       </c>
       <c r="X20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="1">
         <v>0</v>
@@ -11336,7 +11336,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -11348,7 +11348,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
@@ -11375,7 +11375,7 @@
         <v>0</v>
       </c>
       <c r="T21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21" s="1">
         <v>0</v>
@@ -11387,7 +11387,7 @@
         <v>0</v>
       </c>
       <c r="X21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y21" s="1">
         <v>0</v>
@@ -11434,19 +11434,19 @@
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
       </c>
       <c r="I22" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J22" s="1">
         <v>0</v>
       </c>
       <c r="K22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="1">
         <v>0</v>
@@ -11473,19 +11473,19 @@
         <v>0</v>
       </c>
       <c r="T22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22" s="1">
         <v>0</v>
       </c>
       <c r="V22" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W22" s="1">
         <v>0</v>
       </c>
       <c r="X22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y22" s="1">
         <v>0</v>
@@ -11532,7 +11532,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
@@ -11544,7 +11544,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="1">
         <v>0</v>
@@ -11571,7 +11571,7 @@
         <v>0</v>
       </c>
       <c r="T23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="1">
         <v>0</v>
@@ -11583,7 +11583,7 @@
         <v>0</v>
       </c>
       <c r="X23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y23" s="1">
         <v>0</v>

</xml_diff>